<commit_message>
Added BOX, SNOW, WING, BILL, HUBS models
</commit_message>
<xml_diff>
--- a/Cybersecurity/ZScaler.xlsx
+++ b/Cybersecurity/ZScaler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Technology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Cybersecurity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95867C2C-09E4-8748-842A-39EFFF1E99D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BD0CE2-C9B8-C44B-9A51-2C2DE27826F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="28280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28740" yWindow="500" windowWidth="22420" windowHeight="28280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -899,25 +899,9 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="39" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1005,6 +989,24 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="12" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="12" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="11" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2407,11 +2409,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
+      <selection pane="bottomRight" activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2419,7 +2421,8 @@
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="9" width="15" customWidth="1"/>
     <col min="10" max="14" width="19" customWidth="1"/>
-    <col min="15" max="18" width="20" customWidth="1"/>
+    <col min="15" max="17" width="21" customWidth="1"/>
+    <col min="18" max="18" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2450,19 +2453,19 @@
       <c r="I1" s="8">
         <v>2022</v>
       </c>
-      <c r="J1" s="26">
+      <c r="J1" s="21">
         <v>2023</v>
       </c>
-      <c r="K1" s="26">
+      <c r="K1" s="21">
         <v>2024</v>
       </c>
-      <c r="L1" s="26">
+      <c r="L1" s="21">
         <v>2025</v>
       </c>
-      <c r="M1" s="26">
+      <c r="M1" s="21">
         <v>2026</v>
       </c>
-      <c r="N1" s="26">
+      <c r="N1" s="21">
         <v>2027</v>
       </c>
     </row>
@@ -2538,31 +2541,31 @@
       <c r="I3" s="1">
         <v>1090946000</v>
       </c>
-      <c r="J3" s="27">
+      <c r="J3" s="22">
         <v>1561000000</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="22">
         <v>2009000000</v>
       </c>
-      <c r="L3" s="27">
+      <c r="L3" s="22">
         <v>2527000000</v>
       </c>
-      <c r="M3" s="27">
+      <c r="M3" s="22">
         <v>3182000000</v>
       </c>
-      <c r="N3" s="27">
+      <c r="N3" s="22">
         <v>3976000000</v>
       </c>
-      <c r="O3" s="54" t="s">
+      <c r="O3" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="P3" s="55" t="s">
+      <c r="P3" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="Q3" s="55" t="s">
+      <c r="Q3" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="R3" s="55" t="s">
+      <c r="R3" s="45" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2619,19 +2622,19 @@
         <f t="shared" si="0"/>
         <v>0.24952859836580776</v>
       </c>
-      <c r="O4" s="56">
+      <c r="O4" s="46">
         <f>(I4+H4+G4)/3</f>
         <v>0.53520738402986978</v>
       </c>
-      <c r="P4" s="56">
+      <c r="P4" s="46">
         <f>(I20+H20+G20)/3</f>
         <v>1.9422162936945606</v>
       </c>
-      <c r="Q4" s="56">
+      <c r="Q4" s="46">
         <f>(I29+H29+G29)/3</f>
         <v>1.5943240760148953</v>
       </c>
-      <c r="R4" s="56">
+      <c r="R4" s="46">
         <f>(I105+H105+G105)/3</f>
         <v>1.6073435736433679</v>
       </c>
@@ -2711,16 +2714,16 @@
       <c r="I6" s="10">
         <v>848664000</v>
       </c>
-      <c r="O6" s="54" t="s">
+      <c r="O6" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="P6" s="55" t="s">
+      <c r="P6" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="Q6" s="55" t="s">
+      <c r="Q6" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="R6" s="55" t="s">
+      <c r="R6" s="45" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2752,19 +2755,19 @@
       <c r="I7" s="2">
         <v>0.77790000000000004</v>
       </c>
-      <c r="O7" s="56">
+      <c r="O7" s="46">
         <f>I7</f>
         <v>0.77790000000000004</v>
       </c>
-      <c r="P7" s="57">
+      <c r="P7" s="47">
         <f>I21</f>
         <v>-0.25700000000000001</v>
       </c>
-      <c r="Q7" s="57">
+      <c r="Q7" s="47">
         <f>I30</f>
         <v>-0.35770000000000002</v>
       </c>
-      <c r="R7" s="57">
+      <c r="R7" s="47">
         <f>I106/I3</f>
         <v>0.2120471590711181</v>
       </c>
@@ -2836,16 +2839,16 @@
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
-      <c r="O9" s="54" t="s">
+      <c r="O9" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="P9" s="55" t="s">
+      <c r="P9" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="Q9" s="55" t="s">
+      <c r="Q9" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="R9" s="55" t="s">
+      <c r="R9" s="45" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2877,19 +2880,19 @@
       <c r="I10" s="1">
         <v>151735000</v>
       </c>
-      <c r="O10" s="56">
+      <c r="O10" s="46">
         <f>I9</f>
         <v>0.26503511631189813</v>
       </c>
-      <c r="P10" s="57">
+      <c r="P10" s="47">
         <f>I13</f>
         <v>0.81301365970451334</v>
       </c>
-      <c r="Q10" s="57">
+      <c r="Q10" s="47">
         <f>I80</f>
         <v>0.3754191316527124</v>
       </c>
-      <c r="R10" s="57">
+      <c r="R10" s="47">
         <f>I89</f>
         <v>6.3519184267598949E-2</v>
       </c>
@@ -2951,16 +2954,16 @@
       <c r="I12" s="1">
         <v>886954000</v>
       </c>
-      <c r="O12" s="54" t="s">
+      <c r="O12" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="P12" s="55" t="s">
+      <c r="P12" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="Q12" s="55" t="s">
+      <c r="Q12" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="55" t="s">
+      <c r="R12" s="45" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3002,15 +3005,15 @@
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
-      <c r="O13" s="56">
+      <c r="O13" s="46">
         <f>I28/I72</f>
         <v>-0.68075702075702071</v>
       </c>
-      <c r="P13" s="57">
+      <c r="P13" s="47">
         <f>I28/I54</f>
         <v>-0.13777767579293704</v>
       </c>
-      <c r="Q13" s="57">
+      <c r="Q13" s="47">
         <f>I22/(I72+I56+I61)</f>
         <v>-0.20223875895447993</v>
       </c>
@@ -3079,16 +3082,16 @@
       <c r="N15" t="s">
         <v>162</v>
       </c>
-      <c r="O15" s="54" t="s">
+      <c r="O15" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="P15" s="55" t="s">
+      <c r="P15" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="Q15" s="55" t="s">
+      <c r="Q15" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="R15" s="55" t="s">
+      <c r="R15" s="45" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3124,17 +3127,17 @@
         <f>(I35+H35+G35)/3</f>
         <v>4.4726828389374695E-2</v>
       </c>
-      <c r="P16" s="58">
+      <c r="P16" s="48">
         <f>Q101/I3</f>
-        <v>15.582806115059773</v>
-      </c>
-      <c r="Q16" s="58">
+        <v>15.224128966969952</v>
+      </c>
+      <c r="Q16" s="48">
         <f>Q101/I28</f>
-        <v>-43.558694059106585</v>
-      </c>
-      <c r="R16" s="59">
+        <v>-42.556082074828709</v>
+      </c>
+      <c r="R16" s="49">
         <f>Q101/I106</f>
-        <v>73.487455259108117</v>
+        <v>71.795958189960743</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="19" x14ac:dyDescent="0.25">
@@ -3194,7 +3197,7 @@
       <c r="I18" s="1">
         <v>49466000</v>
       </c>
-      <c r="O18" s="54" t="s">
+      <c r="O18" s="44" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3226,7 +3229,7 @@
       <c r="I19" s="10">
         <v>-280368000</v>
       </c>
-      <c r="O19" s="60">
+      <c r="O19" s="50">
         <f>I40-I56-I61</f>
         <v>685617000</v>
       </c>
@@ -3688,31 +3691,31 @@
         <v>106</v>
       </c>
       <c r="B35" s="1"/>
-      <c r="C35" s="23">
+      <c r="C35" s="20">
         <f>(C34-B34)/B34</f>
         <v>1.8717681524154067E-2</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="20">
         <f t="shared" ref="D35:G35" si="9">(D34-C34)/C34</f>
         <v>-1.8373767201281532E-2</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="20">
         <f t="shared" si="9"/>
         <v>-0.37200408957747588</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="20">
         <f t="shared" si="9"/>
         <v>0.93431536763669953</v>
       </c>
-      <c r="G35" s="23">
+      <c r="G35" s="20">
         <f t="shared" si="9"/>
         <v>4.659048605603483E-2</v>
       </c>
-      <c r="H35" s="23">
+      <c r="H35" s="20">
         <f t="shared" ref="H35" si="10">(H34-G34)/G34</f>
         <v>4.8954942276315888E-2</v>
       </c>
-      <c r="I35" s="23">
+      <c r="I35" s="20">
         <f t="shared" ref="I35" si="11">(I34-H34)/H34</f>
         <v>3.8635056835773361E-2</v>
       </c>
@@ -5124,10 +5127,10 @@
       <c r="I83" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P83" s="64" t="s">
+      <c r="P83" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="Q83" s="65"/>
+      <c r="Q83" s="55"/>
     </row>
     <row r="84" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
@@ -5157,10 +5160,10 @@
       <c r="I84" s="1">
         <v>14358000</v>
       </c>
-      <c r="P84" s="66" t="s">
+      <c r="P84" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Q84" s="67"/>
+      <c r="Q84" s="57"/>
     </row>
     <row r="85" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -5190,10 +5193,10 @@
       <c r="I85" s="1">
         <v>251002000</v>
       </c>
-      <c r="P85" s="20" t="s">
+      <c r="P85" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="Q85" s="21">
+      <c r="Q85" s="59">
         <f>I17</f>
         <v>53796000</v>
       </c>
@@ -5226,10 +5229,10 @@
       <c r="I86" s="1">
         <v>156273000</v>
       </c>
-      <c r="P86" s="20" t="s">
+      <c r="P86" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="Q86" s="21">
+      <c r="Q86" s="59">
         <f>I56</f>
         <v>26100000</v>
       </c>
@@ -5262,10 +5265,10 @@
       <c r="I87" s="10">
         <v>321912000</v>
       </c>
-      <c r="P87" s="20" t="s">
+      <c r="P87" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="Q87" s="21">
+      <c r="Q87" s="59">
         <f>I61</f>
         <v>1019622000</v>
       </c>
@@ -5298,15 +5301,15 @@
       <c r="I88" s="1">
         <v>-69296000</v>
       </c>
-      <c r="P88" s="24" t="s">
+      <c r="P88" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="Q88" s="25">
+      <c r="Q88" s="61">
         <f>Q85/(Q86+Q87)</f>
         <v>5.1443882791028593E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
         <v>109</v>
       </c>
@@ -5348,10 +5351,10 @@
       <c r="M89" s="15"/>
       <c r="N89" s="15"/>
       <c r="O89" s="15"/>
-      <c r="P89" s="20" t="s">
+      <c r="P89" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="Q89" s="21">
+      <c r="Q89" s="59">
         <f>I27</f>
         <v>6648000</v>
       </c>
@@ -5384,10 +5387,10 @@
       <c r="I90" s="1">
         <v>-25287000</v>
       </c>
-      <c r="P90" s="20" t="s">
+      <c r="P90" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="Q90" s="21">
+      <c r="Q90" s="59">
         <f>I25</f>
         <v>-383630000</v>
       </c>
@@ -5420,10 +5423,10 @@
       <c r="I91" s="1">
         <v>-844944000</v>
       </c>
-      <c r="P91" s="24" t="s">
+      <c r="P91" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="Q91" s="25">
+      <c r="Q91" s="61">
         <f>Q89/Q90</f>
         <v>-1.7329197403748404E-2</v>
       </c>
@@ -5456,10 +5459,10 @@
       <c r="I92" s="1">
         <v>1334874000</v>
       </c>
-      <c r="P92" s="28" t="s">
+      <c r="P92" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="Q92" s="29">
+      <c r="Q92" s="63">
         <f>Q88*(1-Q91)</f>
         <v>5.2335363991129619E-2</v>
       </c>
@@ -5492,10 +5495,10 @@
       <c r="I93" s="1">
         <v>-21284000</v>
       </c>
-      <c r="P93" s="66" t="s">
+      <c r="P93" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="Q93" s="67"/>
+      <c r="Q93" s="57"/>
     </row>
     <row r="94" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -5525,10 +5528,10 @@
       <c r="I94" s="10">
         <v>374063000</v>
       </c>
-      <c r="P94" s="20" t="s">
+      <c r="P94" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="Q94" s="22">
+      <c r="Q94" s="64">
         <v>4.095E-2</v>
       </c>
     </row>
@@ -5560,10 +5563,10 @@
       <c r="I95" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P95" s="20" t="s">
+      <c r="P95" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="Q95" s="30">
+      <c r="Q95" s="67">
         <v>0.89</v>
       </c>
     </row>
@@ -5595,10 +5598,10 @@
       <c r="I96" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P96" s="20" t="s">
+      <c r="P96" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="Q96" s="22">
+      <c r="Q96" s="64">
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
@@ -5630,10 +5633,10 @@
       <c r="I97" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P97" s="28" t="s">
+      <c r="P97" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="Q97" s="29">
+      <c r="Q97" s="63">
         <f>(Q94)+((Q95)*(Q96-Q94))</f>
         <v>7.9264500000000016E-2</v>
       </c>
@@ -5666,10 +5669,10 @@
       <c r="I98" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P98" s="66" t="s">
+      <c r="P98" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="Q98" s="67"/>
+      <c r="Q98" s="57"/>
     </row>
     <row r="99" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -5699,10 +5702,10 @@
       <c r="I99" s="1">
         <v>41337000</v>
       </c>
-      <c r="P99" s="20" t="s">
+      <c r="P99" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="Q99" s="21">
+      <c r="Q99" s="59">
         <f>Q86+Q87</f>
         <v>1045722000</v>
       </c>
@@ -5735,12 +5738,12 @@
       <c r="I100" s="10">
         <v>41337000</v>
       </c>
-      <c r="P100" s="24" t="s">
+      <c r="P100" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="Q100" s="25">
+      <c r="Q100" s="61">
         <f>Q99/Q103</f>
-        <v>5.7948471111324888E-2</v>
+        <v>5.9232856561068546E-2</v>
       </c>
     </row>
     <row r="101" spans="1:17" ht="20" x14ac:dyDescent="0.25">
@@ -5771,11 +5774,12 @@
       <c r="I101" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P101" s="20" t="s">
+      <c r="P101" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="Q101" s="31">
-        <v>17000000000</v>
+      <c r="Q101" s="36">
+        <f>I34*K116</f>
+        <v>16608702600</v>
       </c>
     </row>
     <row r="102" spans="1:17" ht="20" x14ac:dyDescent="0.25">
@@ -5806,12 +5810,12 @@
       <c r="I102" s="10">
         <v>737312000</v>
       </c>
-      <c r="P102" s="24" t="s">
+      <c r="P102" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="Q102" s="25">
+      <c r="Q102" s="61">
         <f>Q101/Q103</f>
-        <v>0.94205152888867516</v>
+        <v>0.94076714343893142</v>
       </c>
     </row>
     <row r="103" spans="1:17" ht="20" x14ac:dyDescent="0.25">
@@ -5842,12 +5846,12 @@
       <c r="I103" s="1">
         <v>275898000</v>
       </c>
-      <c r="P103" s="28" t="s">
+      <c r="P103" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="Q103" s="32">
+      <c r="Q103" s="65">
         <f>Q99+Q101</f>
-        <v>18045722000</v>
+        <v>17654424600</v>
       </c>
     </row>
     <row r="104" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -5878,10 +5882,10 @@
       <c r="I104" s="11">
         <v>1013210000</v>
       </c>
-      <c r="P104" s="66" t="s">
+      <c r="P104" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="Q104" s="67"/>
+      <c r="Q104" s="57"/>
     </row>
     <row r="105" spans="1:17" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
@@ -5922,12 +5926,12 @@
       <c r="M105" s="15"/>
       <c r="N105" s="15"/>
       <c r="O105" s="15"/>
-      <c r="P105" s="33" t="s">
+      <c r="P105" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="Q105" s="34">
+      <c r="Q105" s="24">
         <f>(Q100*Q92)+(Q102*Q97)</f>
-        <v>7.7703997739937053E-2</v>
+        <v>7.7669410349473098E-2</v>
       </c>
     </row>
     <row r="106" spans="1:17" ht="19" x14ac:dyDescent="0.25">
@@ -5958,33 +5962,33 @@
       <c r="I106" s="1">
         <v>231332000</v>
       </c>
-      <c r="J106" s="35">
+      <c r="J106" s="25">
         <f>I106*(1+$Q$106)</f>
         <v>300011358.18635112</v>
       </c>
-      <c r="K106" s="35">
+      <c r="K106" s="25">
         <f t="shared" ref="K106:N106" si="19">J106*(1+$Q$106)</f>
         <v>389080693.72511834</v>
       </c>
-      <c r="L106" s="35">
+      <c r="L106" s="25">
         <f t="shared" si="19"/>
         <v>504593516.54142296</v>
       </c>
-      <c r="M106" s="35">
+      <c r="M106" s="25">
         <f t="shared" si="19"/>
         <v>654400542.20609057</v>
       </c>
-      <c r="N106" s="35">
+      <c r="N106" s="25">
         <f t="shared" si="19"/>
         <v>848683258.11013532</v>
       </c>
-      <c r="O106" s="36" t="s">
+      <c r="O106" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="P106" s="37" t="s">
+      <c r="P106" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="Q106" s="38">
+      <c r="Q106" s="28">
         <f>(SUM(J4:N4)/5)</f>
         <v>0.29688654482022009</v>
       </c>
@@ -5999,141 +6003,141 @@
       <c r="G107" s="13"/>
       <c r="H107" s="13"/>
       <c r="I107" s="13"/>
-      <c r="J107" s="36"/>
-      <c r="K107" s="36"/>
-      <c r="L107" s="36"/>
-      <c r="M107" s="36"/>
-      <c r="N107" s="39">
+      <c r="J107" s="26"/>
+      <c r="K107" s="26"/>
+      <c r="L107" s="26"/>
+      <c r="M107" s="26"/>
+      <c r="N107" s="29">
         <f>N106*(1+Q107)/(Q108-Q107)</f>
-        <v>16505395735.923687</v>
-      </c>
-      <c r="O107" s="40" t="s">
+        <v>16516234637.732016</v>
+      </c>
+      <c r="O107" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="P107" s="41" t="s">
+      <c r="P107" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="Q107" s="42">
+      <c r="Q107" s="32">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="108" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="J108" s="39">
+      <c r="J108" s="29">
         <f t="shared" ref="J108:L108" si="20">J107+J106</f>
         <v>300011358.18635112</v>
       </c>
-      <c r="K108" s="39">
+      <c r="K108" s="29">
         <f t="shared" si="20"/>
         <v>389080693.72511834</v>
       </c>
-      <c r="L108" s="39">
+      <c r="L108" s="29">
         <f t="shared" si="20"/>
         <v>504593516.54142296</v>
       </c>
-      <c r="M108" s="39">
+      <c r="M108" s="29">
         <f>M107+M106</f>
         <v>654400542.20609057</v>
       </c>
-      <c r="N108" s="39">
+      <c r="N108" s="29">
         <f>N107+N106</f>
-        <v>17354078994.033821</v>
-      </c>
-      <c r="O108" s="40" t="s">
+        <v>17364917895.842152</v>
+      </c>
+      <c r="O108" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="P108" s="43" t="s">
+      <c r="P108" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="Q108" s="44">
+      <c r="Q108" s="34">
         <f>Q105</f>
-        <v>7.7703997739937053E-2</v>
+        <v>7.7669410349473098E-2</v>
       </c>
     </row>
     <row r="109" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="J109" s="62" t="s">
+      <c r="J109" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="K109" s="63"/>
+      <c r="K109" s="53"/>
     </row>
     <row r="110" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="J110" s="45" t="s">
+      <c r="J110" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="K110" s="46">
+      <c r="K110" s="36">
         <f>NPV(Q108,J108,K108,L108,M108,N108)</f>
-        <v>13438866040.819927</v>
+        <v>13448370191.976673</v>
       </c>
     </row>
     <row r="111" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="J111" s="45" t="s">
+      <c r="J111" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="K111" s="46">
+      <c r="K111" s="36">
         <f>I40</f>
         <v>1731339000</v>
       </c>
     </row>
     <row r="112" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="J112" s="45" t="s">
+      <c r="J112" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="K112" s="46">
+      <c r="K112" s="36">
         <f>Q99</f>
         <v>1045722000</v>
       </c>
     </row>
     <row r="113" spans="9:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="J113" s="45" t="s">
+      <c r="J113" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="K113" s="46">
+      <c r="K113" s="36">
         <f>K110+K111-K112</f>
-        <v>14124483040.819927</v>
+        <v>14133987191.976673</v>
       </c>
     </row>
     <row r="114" spans="9:11" ht="20" x14ac:dyDescent="0.25">
       <c r="I114" t="s">
         <v>161</v>
       </c>
-      <c r="J114" s="45" t="s">
+      <c r="J114" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="K114" s="61">
+      <c r="K114" s="51">
         <f>I34*(1+(5*O16))</f>
         <v>172403932.42960474</v>
       </c>
     </row>
     <row r="115" spans="9:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="J115" s="48" t="s">
+      <c r="J115" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="K115" s="49">
+      <c r="K115" s="39">
         <f>K113/K114</f>
-        <v>81.926687180335506</v>
+        <v>81.981814409876094</v>
       </c>
     </row>
     <row r="116" spans="9:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="J116" s="47" t="s">
+      <c r="J116" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="K116" s="50">
+      <c r="K116" s="40">
         <v>117.88</v>
       </c>
     </row>
     <row r="117" spans="9:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="J117" s="51" t="s">
+      <c r="J117" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="K117" s="52">
+      <c r="K117" s="42">
         <f>K115/K116-1</f>
-        <v>-0.30499926043149383</v>
+        <v>-0.30453160493827536</v>
       </c>
     </row>
     <row r="118" spans="9:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="J118" s="51" t="s">
+      <c r="J118" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="K118" s="53" t="str">
+      <c r="K118" s="43" t="str">
         <f>IF(K115&gt;K116,"BUY","SELL")</f>
         <v>SELL</v>
       </c>

</xml_diff>